<commit_message>
ingest auth_groups and clean up the associated permission checks
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="location" sheetId="4" r:id="rId6"/>
     <sheet name="campaign_type" sheetId="9" r:id="rId7"/>
     <sheet name="campaign" sheetId="5" r:id="rId8"/>
-    <sheet name="source-data_pre-campaign-histor" sheetId="6" r:id="rId9"/>
-    <sheet name="source-data_intra-campaign-hist" sheetId="7" r:id="rId10"/>
-    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId11"/>
+    <sheet name="auth_group" sheetId="12" r:id="rId9"/>
+    <sheet name="source-data_pre-campaign-histor" sheetId="6" r:id="rId10"/>
+    <sheet name="source-data_intra-campaign-hist" sheetId="7" r:id="rId11"/>
+    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="1059">
   <si>
     <t>tag_name</t>
   </si>
@@ -3193,6 +3194,24 @@
   </si>
   <si>
     <t>campaign_type_id</t>
+  </si>
+  <si>
+    <t>data_entry</t>
+  </si>
+  <si>
+    <t>source_data</t>
+  </si>
+  <si>
+    <t>manage_system</t>
+  </si>
+  <si>
+    <t>explore_data</t>
+  </si>
+  <si>
+    <t>chart_builder</t>
+  </si>
+  <si>
+    <t>chart_edit</t>
   </si>
 </sst>
 </file>
@@ -3575,7 +3594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -3643,6 +3662,677 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>988</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>989</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>990</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>991</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>992</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>993</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>994</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>995</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>997</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>998</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>999</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>1000</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>1001</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>952</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="N2" s="10">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>967</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+      <c r="L3" s="10">
+        <v>1</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="N3" s="10">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>948</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>949</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0</v>
+      </c>
+      <c r="L4" s="10">
+        <v>1</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N5" s="10">
+        <v>1</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>944</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>945</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N6" s="10">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>956</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>962</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N10" s="10">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N11" s="10">
+        <v>1</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N12" s="10">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N13" s="10">
+        <v>1</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>932</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N14" s="10">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4102,7 +4792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -5696,7 +6386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F442"/>
   <sheetViews>
-    <sheetView topLeftCell="A425" workbookViewId="0">
+    <sheetView topLeftCell="A411" workbookViewId="0">
       <selection activeCell="G442" sqref="G442"/>
     </sheetView>
   </sheetViews>
@@ -15395,668 +16085,71 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>988</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>989</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>990</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>991</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>992</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>993</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>994</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>995</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>996</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>997</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>998</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>999</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>1000</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>1001</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>952</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>953</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K2" s="10">
-        <v>0</v>
-      </c>
-      <c r="L2" s="10">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>1004</v>
-      </c>
-      <c r="N2" s="10">
-        <v>1</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>966</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>967</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0</v>
-      </c>
-      <c r="L3" s="10">
-        <v>1</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>1004</v>
-      </c>
-      <c r="N3" s="10">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>948</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>949</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <v>1</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>1004</v>
-      </c>
-      <c r="N4" s="10">
-        <v>1</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0</v>
-      </c>
-      <c r="L5" s="10">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N5" s="10">
-        <v>1</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>944</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>945</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K6" s="10">
-        <v>0</v>
-      </c>
-      <c r="L6" s="10">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N6" s="10">
-        <v>1</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>956</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>957</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K7" s="10">
-        <v>0</v>
-      </c>
-      <c r="L7" s="10">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N7" s="10">
-        <v>1</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>960</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>961</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>1004</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N8" s="10">
-        <v>0.98</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>962</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>963</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>1004</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K9" s="10">
-        <v>0</v>
-      </c>
-      <c r="L9" s="10">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N9" s="10">
-        <v>0.98</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K10" s="10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N10" s="10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K11" s="10">
-        <v>0</v>
-      </c>
-      <c r="L11" s="10">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N11" s="10">
-        <v>1</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K12" s="10">
-        <v>0</v>
-      </c>
-      <c r="L12" s="10">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N12" s="10">
-        <v>1</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K13" s="10">
-        <v>0</v>
-      </c>
-      <c r="L13" s="10">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N13" s="10">
-        <v>1</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>932</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>933</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="K14" s="10">
-        <v>0</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="N14" s="10">
-        <v>1</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>1003</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- fix maximum recusion error in urls after changing custom_dashboard view name    - add doc_detail_types to initial_data ingest    - working through source_data to handle a world with no document_ids
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="campaign_type" sheetId="9" r:id="rId7"/>
     <sheet name="campaign" sheetId="5" r:id="rId8"/>
     <sheet name="auth_group" sheetId="12" r:id="rId9"/>
-    <sheet name="source-data_pre-campaign-histor" sheetId="6" r:id="rId10"/>
-    <sheet name="source-data_intra-campaign-hist" sheetId="7" r:id="rId11"/>
-    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId12"/>
+    <sheet name="doc_detail_type" sheetId="15" r:id="rId10"/>
+    <sheet name="source-data_pre-campaign-histor" sheetId="6" r:id="rId11"/>
+    <sheet name="source-data_intra-campaign-hist" sheetId="7" r:id="rId12"/>
+    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId13"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="1070">
   <si>
     <t>tag_name</t>
   </si>
@@ -3212,6 +3213,39 @@
   </si>
   <si>
     <t>chart_edit</t>
+  </si>
+  <si>
+    <t>location_column</t>
+  </si>
+  <si>
+    <t>uq_id_column</t>
+  </si>
+  <si>
+    <t>submission_count</t>
+  </si>
+  <si>
+    <t>submission_processed_count</t>
+  </si>
+  <si>
+    <t>submission_to_process_count</t>
+  </si>
+  <si>
+    <t>doc_datapoint_count</t>
+  </si>
+  <si>
+    <t>datapoint_count</t>
+  </si>
+  <si>
+    <t>agg_datapoint_count</t>
+  </si>
+  <si>
+    <t>calc_datapoint_count</t>
+  </si>
+  <si>
+    <t>date_column</t>
+  </si>
+  <si>
+    <t>campaign_column</t>
   </si>
 </sst>
 </file>
@@ -3662,6 +3696,120 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4331,7 +4479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -4792,7 +4940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -16087,7 +16235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix python tests after schema changes
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,8 @@
     <sheet name="cache_job" sheetId="17" r:id="rId13"/>
     <sheet name="source-data_intra-campaign-hist" sheetId="7" r:id="rId14"/>
     <sheet name="source-data_pre-campaign-histor" sheetId="6" r:id="rId15"/>
-    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId16"/>
+    <sheet name="custom_chart" sheetId="19" r:id="rId16"/>
+    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId17"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2491" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2500" uniqueCount="1126">
   <si>
     <t>tag_name</t>
   </si>
@@ -3393,13 +3394,37 @@
   </si>
   <si>
     <t>location_attribute_type</t>
+  </si>
+  <si>
+    <t>chart_title</t>
+  </si>
+  <si>
+    <t>chart_json</t>
+  </si>
+  <si>
+    <t>{"startDate":"2015-01-01","z":0,"endDate":"2015-01-01","countries":[],"location_id":1,"timeRange":null,"locations":"sublocations","y":0,"x":21,"indicators":[21],"title":"Percent Miissed Children ( Outside Sample ) ","location_ids":[432,428,429,40,424,37,351,431,47,50,422,415,45,414,420,426],"yFormat":"%","type":"ChoroplethMap","groupBy":"indicator","xFormat":"%"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent Missed Children ( Outside Sampe ) </t>
+  </si>
+  <si>
+    <t>{"startDate":"2015-02-28","z":0,"endDate":"2016-02-29","countries":[],"location_id":1,"timeRange":null,"locations":"selected","y":20,"x":13,"indicators":[13,20],"title":"Post Campaign Table","location_ids":[33,424,1,432,428,429,40,37,351,431,47,50,422,415,45,414,420,426],"yFormat":",.0f","type":"TableChart","groupBy":"indicator","xFormat":",.0f"}</t>
+  </si>
+  <si>
+    <t>Post Campaign Tabe</t>
+  </si>
+  <si>
+    <t>{"countries":[],"endDate":"2015-01-01","groupBy":"indicator","indicators":[21],"location_id":1,"location_ids":[424],"locations":"sublocations","startDate":"2015-01-01","timeRange":null,"title":"Percent Miissed Children Line Chart","type":"LineChart","x":21,"xFormat":"%","y":0,"yFormat":"%","z":0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trend -- Percent Missed Children ( Outside Sampe ) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3433,6 +3458,16 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF303942"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -3470,7 +3505,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3496,6 +3531,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -39279,11 +39316,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.621616319448</v>
+        <v>42429.656739120372</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.621616319448</v>
+        <v>42429.656739120372</v>
       </c>
       <c r="D2" t="s">
         <v>1110</v>
@@ -39295,11 +39332,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.621616319448</v>
+        <v>42429.656739120372</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.621616319448</v>
+        <v>42429.656739120372</v>
       </c>
       <c r="D3" t="s">
         <v>1110</v>
@@ -39945,8 +39982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -40702,6 +40739,68 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="G9" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>

</xml_diff>

<commit_message>
Save chart title in its own column.
Also, renamed 'chart_title' column to 'title'
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/rhizome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Dropbox/vhosts/clients/rhizome/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3396,9 +3396,6 @@
     <t>location_attribute_type</t>
   </si>
   <si>
-    <t>chart_title</t>
-  </si>
-  <si>
     <t>chart_json</t>
   </si>
   <si>
@@ -3418,6 +3415,9 @@
   </si>
   <si>
     <t xml:space="preserve">Trend -- Percent Missed Children ( Outside Sampe ) </t>
+  </si>
+  <si>
+    <t>title</t>
   </si>
 </sst>
 </file>
@@ -39316,11 +39316,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.656739120372</v>
+        <v>42429.474703125001</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.656739120372</v>
+        <v>42429.474703125001</v>
       </c>
       <c r="D2" t="s">
         <v>1110</v>
@@ -39332,11 +39332,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.656739120372</v>
+        <v>42429.474703125001</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.656739120372</v>
+        <v>42429.474703125001</v>
       </c>
       <c r="D3" t="s">
         <v>1110</v>
@@ -40743,7 +40743,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -40753,10 +40753,10 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C1" t="s">
         <v>1118</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -40764,10 +40764,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="C2" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -40775,10 +40775,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C3" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -40786,10 +40786,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fix custom chart save to put title into the appropriate field
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Dropbox/vhosts/clients/rhizome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/rhizome/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="indicator" sheetId="3" r:id="rId4"/>
     <sheet name="indicator_to_tag" sheetId="10" r:id="rId5"/>
     <sheet name="location" sheetId="4" r:id="rId6"/>
-    <sheet name="campaign_type" sheetId="9" r:id="rId7"/>
-    <sheet name="campaign" sheetId="5" r:id="rId8"/>
-    <sheet name="auth_group" sheetId="12" r:id="rId9"/>
-    <sheet name="doc_detail_type" sheetId="15" r:id="rId10"/>
-    <sheet name="source_object_map" sheetId="16" r:id="rId11"/>
-    <sheet name="cache_job" sheetId="17" r:id="rId12"/>
-    <sheet name="source-data_intra-campaign-hist" sheetId="7" r:id="rId13"/>
-    <sheet name="source-data_pre-campaign-histor" sheetId="6" r:id="rId14"/>
-    <sheet name="custom_chart" sheetId="19" r:id="rId15"/>
-    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId16"/>
+    <sheet name="datapoint_with_computed" sheetId="20" r:id="rId7"/>
+    <sheet name="campaign_type" sheetId="9" r:id="rId8"/>
+    <sheet name="campaign" sheetId="5" r:id="rId9"/>
+    <sheet name="auth_group" sheetId="12" r:id="rId10"/>
+    <sheet name="doc_detail_type" sheetId="15" r:id="rId11"/>
+    <sheet name="source_object_map" sheetId="16" r:id="rId12"/>
+    <sheet name="cache_job" sheetId="17" r:id="rId13"/>
+    <sheet name="custom_chart" sheetId="19" r:id="rId14"/>
+    <sheet name="source-data_intra-campaign-hist" sheetId="7" r:id="rId15"/>
+    <sheet name="source-data_pre-campaign-histor" sheetId="6" r:id="rId16"/>
+    <sheet name="source-data_post-campaign-histo" sheetId="8" r:id="rId17"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2413" uniqueCount="1130">
   <si>
     <t>tag_name</t>
   </si>
@@ -3408,6 +3409,27 @@
   </si>
   <si>
     <t>lpd_status</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>cache_job_Id</t>
+  </si>
+  <si>
+    <t>campaign_id</t>
+  </si>
+  <si>
+    <t>location_id</t>
+  </si>
+  <si>
+    <t>indicator_name</t>
+  </si>
+  <si>
+    <t>location_name</t>
+  </si>
+  <si>
+    <t>campaign_name</t>
   </si>
 </sst>
 </file>
@@ -3484,8 +3506,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3524,15 +3548,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3878,6 +3904,80 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3990,7 +4090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8616"/>
   <sheetViews>
@@ -39199,7 +39299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -39232,11 +39332,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42430.462691782406</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42430.462691782406</v>
       </c>
       <c r="D2" t="s">
         <v>1110</v>
@@ -39248,645 +39348,14 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42430.462691782406</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42430.462691782406</v>
       </c>
       <c r="D3" t="s">
         <v>1110</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>1055</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>1004</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>1005</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>1006</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>1007</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>1008</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>1009</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>1010</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>1011</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>9</v>
-      </c>
-      <c r="B2" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>953</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>952</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.93175128299999999</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.45751116400000003</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0.82776713800000001</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0.68092942400000001</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0.30315546799999998</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0.132785559</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0.28942163300000001</v>
-      </c>
-      <c r="M2" s="6">
-        <v>5</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>10</v>
-      </c>
-      <c r="B3" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>967</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>966</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0.92731706999999997</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.684749108</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0.78842665300000003</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.86370060400000004</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0.50499575600000002</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0.87669438600000005</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.19922045199999999</v>
-      </c>
-      <c r="M3" s="6">
-        <v>7</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>11</v>
-      </c>
-      <c r="B4" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>949</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>948</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.77017539000000002</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.60959730599999995</v>
-      </c>
-      <c r="H4" s="6">
-        <v>8.6094840000000006E-3</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.21138432300000001</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0.475142974</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0.35318346099999998</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.96924487299999995</v>
-      </c>
-      <c r="M4" s="6">
-        <v>8</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>12</v>
-      </c>
-      <c r="B5" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0.67949911799999996</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.98780689700000002</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0.342283271</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0.30764573000000001</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0.42363846100000002</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0.53742198399999996</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0.60442163500000001</v>
-      </c>
-      <c r="M5" s="6">
-        <v>7</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>13</v>
-      </c>
-      <c r="B6" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>945</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>944</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.36322991199999999</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0.585966498</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0.28058723299999999</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.57867705300000005</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0.29612353400000002</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0.502473104</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0.96767113800000004</v>
-      </c>
-      <c r="M6" s="6">
-        <v>6</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>14</v>
-      </c>
-      <c r="B7" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>957</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>956</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0.86703272099999995</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0.96711685800000002</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0.46170325800000001</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0.17533649300000001</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0.60445965599999996</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0.89186230099999997</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0.53500187600000004</v>
-      </c>
-      <c r="M7" s="6">
-        <v>6</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>15</v>
-      </c>
-      <c r="B8" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>961</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0.46587564199999998</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.22875558200000001</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.41388356900000001</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0.340464712</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0.15157773399999999</v>
-      </c>
-      <c r="K8" s="6">
-        <v>6.6392779999999998E-2</v>
-      </c>
-      <c r="L8" s="6">
-        <v>0.14471081699999999</v>
-      </c>
-      <c r="M8" s="6">
-        <v>3</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>16</v>
-      </c>
-      <c r="B9" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>963</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>962</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0.46365853499999998</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.342374554</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0.394213327</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0.43185030200000002</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0.25249787800000001</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0.43834719300000002</v>
-      </c>
-      <c r="L9" s="6">
-        <v>9.9610225999999996E-2</v>
-      </c>
-      <c r="M9" s="6">
-        <v>4</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>17</v>
-      </c>
-      <c r="B10" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0.38508769500000001</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.30479865299999997</v>
-      </c>
-      <c r="H10" s="6">
-        <v>4.3047420000000003E-3</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.10569216200000001</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0.237571487</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0.176591731</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0.48462243700000002</v>
-      </c>
-      <c r="M10" s="6">
-        <v>4</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>18</v>
-      </c>
-      <c r="B11" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0.33974955899999998</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.49390344899999999</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0.17114163600000001</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.153822865</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0.211819231</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0.26871099199999998</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0.30221081799999999</v>
-      </c>
-      <c r="M11" s="6">
-        <v>4</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>19</v>
-      </c>
-      <c r="B12" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0.18161495599999999</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0.292983249</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0.14029361700000001</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0.28933852700000001</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0.14806176700000001</v>
-      </c>
-      <c r="K12" s="6">
-        <v>0.251236552</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0.48383556900000002</v>
-      </c>
-      <c r="M12" s="6">
-        <v>3</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>20</v>
-      </c>
-      <c r="B13" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.43351636100000002</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0.48355842900000001</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0.230851629</v>
-      </c>
-      <c r="I13" s="6">
-        <v>8.7668247000000005E-2</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0.30222982799999998</v>
-      </c>
-      <c r="K13" s="6">
-        <v>0.44593115100000003</v>
-      </c>
-      <c r="L13" s="6">
-        <v>0.26750093800000002</v>
-      </c>
-      <c r="M13" s="6">
-        <v>3</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>21</v>
-      </c>
-      <c r="B14" s="15">
-        <v>42370</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>1113</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>933</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>932</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.23293782099999999</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0.11437779100000001</v>
-      </c>
-      <c r="H14" s="6">
-        <v>0.20694178499999999</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0.170232356</v>
-      </c>
-      <c r="J14" s="6">
-        <v>7.5788866999999996E-2</v>
-      </c>
-      <c r="K14" s="6">
-        <v>3.3196389999999999E-2</v>
-      </c>
-      <c r="L14" s="6">
-        <v>7.2355407999999996E-2</v>
-      </c>
-      <c r="M14" s="6">
-        <v>2</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>1003</v>
       </c>
     </row>
   </sheetData>
@@ -39895,766 +39364,6 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1055</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1064</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>988</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>989</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>990</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>991</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>992</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>993</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>994</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>995</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>996</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>997</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>998</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>999</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>952</v>
-      </c>
-      <c r="C2" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>953</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M2" s="10">
-        <v>0</v>
-      </c>
-      <c r="N2" s="10">
-        <v>1</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="P2" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>966</v>
-      </c>
-      <c r="C3" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>967</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M3" s="10">
-        <v>0</v>
-      </c>
-      <c r="N3" s="10">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="P3" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>948</v>
-      </c>
-      <c r="C4" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>949</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M4" s="10">
-        <v>0</v>
-      </c>
-      <c r="N4" s="10">
-        <v>1</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="P4" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M5" s="10">
-        <v>0</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P5" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>944</v>
-      </c>
-      <c r="C6" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>945</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M6" s="10">
-        <v>0</v>
-      </c>
-      <c r="N6" s="10">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P6" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>956</v>
-      </c>
-      <c r="C7" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>957</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M7" s="10">
-        <v>0</v>
-      </c>
-      <c r="N7" s="10">
-        <v>0</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P7" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>960</v>
-      </c>
-      <c r="C8" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>961</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M8" s="10">
-        <v>0</v>
-      </c>
-      <c r="N8" s="10">
-        <v>0</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P8" s="10">
-        <v>0.98</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>962</v>
-      </c>
-      <c r="C9" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>963</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>1003</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M9" s="10">
-        <v>0</v>
-      </c>
-      <c r="N9" s="10">
-        <v>0</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P9" s="10">
-        <v>0.98</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C10" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M10" s="10">
-        <v>0</v>
-      </c>
-      <c r="N10" s="10">
-        <v>0</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P10" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M11" s="10">
-        <v>0</v>
-      </c>
-      <c r="N11" s="10">
-        <v>0</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P11" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="C12" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M12" s="10">
-        <v>0</v>
-      </c>
-      <c r="N12" s="10">
-        <v>0</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P12" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C13" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M13" s="10">
-        <v>0</v>
-      </c>
-      <c r="N13" s="10">
-        <v>0</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P13" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>932</v>
-      </c>
-      <c r="C14" s="16">
-        <v>42370</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>933</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0</v>
-      </c>
-      <c r="N14" s="10">
-        <v>0</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>1002</v>
-      </c>
-      <c r="P14" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -40716,12 +39425,1403 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1007</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>1010</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>1011</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>9</v>
+      </c>
+      <c r="B2" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>953</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.93175128299999999</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.45751116400000003</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.82776713800000001</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.68092942400000001</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0.30315546799999998</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0.132785559</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.28942163300000001</v>
+      </c>
+      <c r="M2" s="6">
+        <v>5</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>10</v>
+      </c>
+      <c r="B3" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>967</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>966</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.92731706999999997</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.684749108</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.78842665300000003</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.86370060400000004</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.50499575600000002</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.87669438600000005</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.19922045199999999</v>
+      </c>
+      <c r="M3" s="6">
+        <v>7</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>11</v>
+      </c>
+      <c r="B4" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>949</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>948</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.77017539000000002</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.60959730599999995</v>
+      </c>
+      <c r="H4" s="6">
+        <v>8.6094840000000006E-3</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.21138432300000001</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.475142974</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.35318346099999998</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.96924487299999995</v>
+      </c>
+      <c r="M4" s="6">
+        <v>8</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>12</v>
+      </c>
+      <c r="B5" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.67949911799999996</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.98780689700000002</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.342283271</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.30764573000000001</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.42363846100000002</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.53742198399999996</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.60442163500000001</v>
+      </c>
+      <c r="M5" s="6">
+        <v>7</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>13</v>
+      </c>
+      <c r="B6" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>945</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>944</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.36322991199999999</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.585966498</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.28058723299999999</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.57867705300000005</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.29612353400000002</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.502473104</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.96767113800000004</v>
+      </c>
+      <c r="M6" s="6">
+        <v>6</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>957</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>956</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.86703272099999995</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.96711685800000002</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.46170325800000001</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.17533649300000001</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.60445965599999996</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.89186230099999997</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0.53500187600000004</v>
+      </c>
+      <c r="M7" s="6">
+        <v>6</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>15</v>
+      </c>
+      <c r="B8" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>961</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.46587564199999998</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.22875558200000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.41388356900000001</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.340464712</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.15157773399999999</v>
+      </c>
+      <c r="K8" s="6">
+        <v>6.6392779999999998E-2</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0.14471081699999999</v>
+      </c>
+      <c r="M8" s="6">
+        <v>3</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>16</v>
+      </c>
+      <c r="B9" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>963</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>962</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.46365853499999998</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.342374554</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.394213327</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.43185030200000002</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.25249787800000001</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.43834719300000002</v>
+      </c>
+      <c r="L9" s="6">
+        <v>9.9610225999999996E-2</v>
+      </c>
+      <c r="M9" s="6">
+        <v>4</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.38508769500000001</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.30479865299999997</v>
+      </c>
+      <c r="H10" s="6">
+        <v>4.3047420000000003E-3</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.10569216200000001</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.237571487</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.176591731</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.48462243700000002</v>
+      </c>
+      <c r="M10" s="6">
+        <v>4</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>18</v>
+      </c>
+      <c r="B11" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.33974955899999998</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.49390344899999999</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.17114163600000001</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.153822865</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.211819231</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.26871099199999998</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0.30221081799999999</v>
+      </c>
+      <c r="M11" s="6">
+        <v>4</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>19</v>
+      </c>
+      <c r="B12" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.18161495599999999</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.292983249</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.14029361700000001</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.28933852700000001</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.14806176700000001</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.251236552</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.48383556900000002</v>
+      </c>
+      <c r="M12" s="6">
+        <v>3</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>20</v>
+      </c>
+      <c r="B13" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.43351636100000002</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.48355842900000001</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.230851629</v>
+      </c>
+      <c r="I13" s="6">
+        <v>8.7668247000000005E-2</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.30222982799999998</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.44593115100000003</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0.26750093800000002</v>
+      </c>
+      <c r="M13" s="6">
+        <v>3</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>21</v>
+      </c>
+      <c r="B14" s="15">
+        <v>42370</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>932</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.23293782099999999</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.11437779100000001</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.20694178499999999</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.170232356</v>
+      </c>
+      <c r="J14" s="6">
+        <v>7.5788866999999996E-2</v>
+      </c>
+      <c r="K14" s="6">
+        <v>3.3196389999999999E-2</v>
+      </c>
+      <c r="L14" s="6">
+        <v>7.2355407999999996E-2</v>
+      </c>
+      <c r="M14" s="6">
+        <v>2</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>988</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>989</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>990</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>991</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>992</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>993</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>994</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>995</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>997</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>998</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>999</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>1000</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>952</v>
+      </c>
+      <c r="C2" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M2" s="10">
+        <v>0</v>
+      </c>
+      <c r="N2" s="10">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="C3" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>967</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="P3" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>948</v>
+      </c>
+      <c r="C4" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>949</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M4" s="10">
+        <v>0</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>944</v>
+      </c>
+      <c r="C6" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>945</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M6" s="10">
+        <v>0</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P6" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>956</v>
+      </c>
+      <c r="C7" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P7" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="C8" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>961</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>962</v>
+      </c>
+      <c r="C9" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P9" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M10" s="10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P10" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0</v>
+      </c>
+      <c r="N11" s="10">
+        <v>0</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P11" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P12" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0</v>
+      </c>
+      <c r="N13" s="10">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P13" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>932</v>
+      </c>
+      <c r="C14" s="16">
+        <v>42370</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="M14" s="10">
+        <v>0</v>
+      </c>
+      <c r="N14" s="10">
+        <v>0</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="P14" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -41354,7 +41454,7 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -42143,10 +42243,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -42177,23 +42277,23 @@
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -42201,15 +42301,15 @@
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -42217,103 +42317,103 @@
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -42321,7 +42421,7 @@
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -42329,53 +42429,64 @@
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>27</v>
+      </c>
+      <c r="B29">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B28">
+    <sortCondition ref="B2:B28"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -42384,8 +42495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I442"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E11:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -52059,6 +52170,541 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>VLOOKUP(A2,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Evening meeting</v>
+      </c>
+      <c r="G2" t="str">
+        <f>VLOOKUP(E2,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H2" t="str">
+        <f>VLOOKUP(D2,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <f>VLOOKUP(A3,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>FLW training plan</v>
+      </c>
+      <c r="G3" t="str">
+        <f>VLOOKUP(E3,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H3" t="str">
+        <f>VLOOKUP(D3,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <f>VLOOKUP(A4,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Percent volunteers trained</v>
+      </c>
+      <c r="G4" t="str">
+        <f>VLOOKUP(E4,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H4" t="str">
+        <f>VLOOKUP(D4,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <f>VLOOKUP(A5,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Percent vx team supervised</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(E5,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H5" t="str">
+        <f>VLOOKUP(D5,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <f>VLOOKUP(A6,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Percent vx team trained</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(E6,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H6" t="str">
+        <f>VLOOKUP(D6,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <f>VLOOKUP(A7,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Percent vx team using stage 3 or 4 vaccines</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(E7,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H7" t="str">
+        <f>VLOOKUP(D7,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>-1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <f>VLOOKUP(A8,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Percent FLWs (operation) paid</v>
+      </c>
+      <c r="G8" t="str">
+        <f>VLOOKUP(E8,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H8" t="str">
+        <f>VLOOKUP(D8,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>-1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <f>VLOOKUP(A9,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Out of House Missed Children</v>
+      </c>
+      <c r="G9" t="str">
+        <f>VLOOKUP(E9,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H9" t="str">
+        <f>VLOOKUP(D9,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
+        <f>VLOOKUP(A10,indicator!$A$2:$C$28,3,FALSE)</f>
+        <v>Percent FLWs (social mobilisers) paid</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP(E10,location!$A$2:$D$442,4,FALSE)</f>
+        <v>Afghanistan</v>
+      </c>
+      <c r="H10" t="str">
+        <f>VLOOKUP(D10,campaign!$A$2:$D$14,4,FALSE)</f>
+        <v>Afghanistan NID January 2015</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="6:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="6:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -52116,57 +52762,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>1020</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1021</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1048</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1045</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1046</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
         <v>42005</v>
       </c>
-      <c r="B2" s="12">
+      <c r="C2" s="12">
         <v>42035</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1024</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -52176,20 +52825,23 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="12">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
         <v>42036</v>
       </c>
-      <c r="B3" s="12">
+      <c r="C3" s="12">
         <v>42063</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1028</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="E3">
         <v>1</v>
       </c>
@@ -52199,20 +52851,23 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="12">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
         <v>42064</v>
       </c>
-      <c r="B4" s="12">
+      <c r="C4" s="12">
         <v>42094</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>1029</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
       <c r="E4">
         <v>1</v>
       </c>
@@ -52222,20 +52877,23 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
         <v>42095</v>
       </c>
-      <c r="B5" s="12">
+      <c r="C5" s="12">
         <v>42124</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>1030</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
       <c r="E5">
         <v>1</v>
       </c>
@@ -52245,20 +52903,23 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="12">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
         <v>42125</v>
       </c>
-      <c r="B6" s="12">
+      <c r="C6" s="12">
         <v>42155</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1031</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -52268,20 +52929,23 @@
       <c r="G6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="12">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
         <v>42156</v>
       </c>
-      <c r="B7" s="12">
+      <c r="C7" s="12">
         <v>42185</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>1026</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -52291,20 +52955,23 @@
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="12">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
         <v>42186</v>
       </c>
-      <c r="B8" s="12">
+      <c r="C8" s="12">
         <v>42216</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>1032</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
       <c r="E8">
         <v>1</v>
       </c>
@@ -52314,20 +52981,23 @@
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="12">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
         <v>42217</v>
       </c>
-      <c r="B9" s="12">
+      <c r="C9" s="12">
         <v>42247</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>1033</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
       <c r="E9">
         <v>1</v>
       </c>
@@ -52337,20 +53007,23 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
         <v>42248</v>
       </c>
-      <c r="B10" s="12">
+      <c r="C10" s="12">
         <v>42277</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>1034</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
       <c r="E10">
         <v>1</v>
       </c>
@@ -52360,20 +53033,23 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
         <v>42278</v>
       </c>
-      <c r="B11" s="12">
+      <c r="C11" s="12">
         <v>42308</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>1022</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
       <c r="E11">
         <v>1</v>
       </c>
@@ -52383,20 +53059,23 @@
       <c r="G11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
         <v>42309</v>
       </c>
-      <c r="B12" s="12">
+      <c r="C12" s="12">
         <v>42338</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>1027</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
       <c r="E12">
         <v>1</v>
       </c>
@@ -52406,20 +53085,23 @@
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
         <v>42339</v>
       </c>
-      <c r="B13" s="12">
+      <c r="C13" s="12">
         <v>42369</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>1023</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
       <c r="E13">
         <v>1</v>
       </c>
@@ -52429,20 +53111,23 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12">
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
         <v>42370</v>
       </c>
-      <c r="B14" s="12">
+      <c r="C14" s="12">
         <v>42398</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>1025</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
       <c r="E14">
         <v>1</v>
       </c>
@@ -52452,85 +53137,14 @@
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C15">
-    <sortCondition ref="A2:A15"/>
+  <sortState ref="B2:D15">
+    <sortCondition ref="B2:B15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update intial data to match new attirube names
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" firstSheet="1" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -3386,21 +3386,12 @@
     <t>chart_json</t>
   </si>
   <si>
-    <t>{"startDate":"2015-01-01","z":0,"endDate":"2015-01-01","countries":[],"location_id":1,"timeRange":null,"locations":"sublocations","y":0,"x":21,"indicators":[21],"title":"Percent Miissed Children ( Outside Sample ) ","location_ids":[432,428,429,40,424,37,351,431,47,50,422,415,45,414,420,426],"yFormat":"%","type":"ChoroplethMap","groupBy":"indicator","xFormat":"%"}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Percent Missed Children ( Outside Sampe ) </t>
   </si>
   <si>
-    <t>{"startDate":"2015-02-28","z":0,"endDate":"2016-02-29","countries":[],"location_id":1,"timeRange":null,"locations":"selected","y":20,"x":13,"indicators":[13,20],"title":"Post Campaign Table","location_ids":[33,424,1,432,428,429,40,37,351,431,47,50,422,415,45,414,420,426],"yFormat":",.0f","type":"TableChart","groupBy":"indicator","xFormat":",.0f"}</t>
-  </si>
-  <si>
     <t>Post Campaign Tabe</t>
   </si>
   <si>
-    <t>{"countries":[],"endDate":"2015-01-01","groupBy":"indicator","indicators":[21],"location_id":1,"location_ids":[424],"locations":"sublocations","startDate":"2015-01-01","timeRange":null,"title":"Percent Miissed Children Line Chart","type":"LineChart","x":21,"xFormat":"%","y":0,"yFormat":"%","z":0}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trend -- Percent Missed Children ( Outside Sampe ) </t>
   </si>
   <si>
@@ -3408,6 +3399,15 @@
   </si>
   <si>
     <t>lpd_status</t>
+  </si>
+  <si>
+    <t>{"countries":[],"endDate":"2015-01-01","groupBy":"indicator","indicator_ids":[21],"location_id":1,"location_ids":[424],"location_depth":"sublocations","startDate":"2015-01-01","timeRange":null,"title":"Percent Miissed Children Line Chart","type":"LineChart","x":21,"xFormat":"%","y":0,"yFormat":"%","z":0}</t>
+  </si>
+  <si>
+    <t>{"startDate":"2015-01-01","z":0,"endDate":"2015-01-01","countries":[],"location_id":1,"timeRange":null,"location_depth":"sublocations","y":0,"x":21,"indicator_ids":[21],"title":"Percent Miissed Children ( Outside Sample ) ","location_ids":[432,428,429,40,424,37,351,431,47,50,422,415,45,414,420,426],"yFormat":"%","type":"ChoroplethMap","groupBy":"indicator","xFormat":"%"}</t>
+  </si>
+  <si>
+    <t>{"startDate":"2015-02-28","z":0,"endDate":"2016-02-29","countries":[],"location_id":1,"timeRange":null,"location_depth":"selected","y":20,"x":13,"indicator_ids":[13,20],"title":"Post Campaign Table","location_ids":[33,424,1,432,428,429,40,37,351,431,47,50,422,415,45,414,420,426],"yFormat":",.0f","type":"TableChart","groupBy":"indicator","xFormat":",.0f"}</t>
   </si>
 </sst>
 </file>
@@ -39232,11 +39232,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42429.954942939818</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42429.954942939818</v>
       </c>
       <c r="D2" t="s">
         <v>1110</v>
@@ -39248,11 +39248,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42429.954942939818</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42429.506537037036</v>
+        <v>42429.954942939818</v>
       </c>
       <c r="D3" t="s">
         <v>1110</v>
@@ -40658,8 +40658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -40669,7 +40669,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="C1" t="s">
         <v>1114</v>
@@ -40680,10 +40680,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C2" t="s">
-        <v>1115</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -40691,10 +40691,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C3" t="s">
-        <v>1117</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -40702,10 +40702,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>1120</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31" x14ac:dyDescent="0.35">
@@ -42384,7 +42384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I442"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
@@ -42414,7 +42414,7 @@
         <v>1045</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update chart store and chart actions
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/rhizome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Dropbox/vhosts/clients/rhizome/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -3368,21 +3368,12 @@
     <t>chart_json</t>
   </si>
   <si>
-    <t>{"startDate":"2015-01-01","z":0,"endDate":"2015-01-01","countries":[],"location_id":1,"timeRange":null,"locations":"sublocations","y":0,"x":21,"indicators":[21],"title":"Percent Miissed Children ( Outside Sample ) ","location_ids":[432,428,429,40,424,37,351,431,47,50,422,415,45,414,420,426],"yFormat":"%","type":"ChoroplethMap","groupBy":"indicator","xFormat":"%"}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Percent Missed Children ( Outside Sampe ) </t>
   </si>
   <si>
-    <t>{"startDate":"2015-02-28","z":0,"endDate":"2016-02-29","countries":[],"location_id":1,"timeRange":null,"locations":"selected","y":20,"x":13,"indicators":[13,20],"title":"Post Campaign Table","location_ids":[33,424,1,432,428,429,40,37,351,431,47,50,422,415,45,414,420,426],"yFormat":",.0f","type":"TableChart","groupBy":"indicator","xFormat":",.0f"}</t>
-  </si>
-  <si>
     <t>Post Campaign Tabe</t>
   </si>
   <si>
-    <t>{"countries":[],"endDate":"2015-01-01","groupBy":"indicator","indicators":[21],"location_id":1,"location_ids":[424],"locations":"sublocations","startDate":"2015-01-01","timeRange":null,"title":"Percent Miissed Children Line Chart","type":"LineChart","x":21,"xFormat":"%","y":0,"yFormat":"%","z":0}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trend -- Percent Missed Children ( Outside Sampe ) </t>
   </si>
   <si>
@@ -3417,6 +3408,15 @@
   </si>
   <si>
     <t>Integer value cooresponding to the prerformance of a district</t>
+  </si>
+  <si>
+    <t>{"startDate":"2015-01-01","z":0,"endDate":"2015-01-01","countries":[],"location_id":1,"timeRange":null,"locations":"sublocations","y":0,"x":21,"indicator_ids":[21],"title":"Percent Miissed Children ( Outside Sample ) ","location_ids":[432,428,429,40,424,37,351,431,47,50,422,415,45,414,420,426],"yFormat":"%","type":"ChoroplethMap","groupBy":"indicator","xFormat":"%"}</t>
+  </si>
+  <si>
+    <t>{"countries":[],"endDate":"2015-01-01","groupBy":"indicator","indicator_ids":[21],"location_id":1,"location_ids":[424],"locations":"sublocations","startDate":"2015-01-01","timeRange":null,"title":"Percent Miissed Children Line Chart","type":"LineChart","x":21,"xFormat":"%","y":0,"yFormat":"%","z":0}</t>
+  </si>
+  <si>
+    <t>{"startDate":"2015-02-28","z":0,"endDate":"2016-02-29","countries":[],"location_id":1,"timeRange":null,"locations":"selected","y":20,"x":13,"indicator_ids":[13,20],"title":"Post Campaign Table","location_ids":[33,424,1,432,428,429,40,37,351,431,47,50,422,415,45,414,420,426],"yFormat":",.0f","type":"TableChart","groupBy":"indicator","xFormat":",.0f"}</t>
   </si>
 </sst>
 </file>
@@ -39249,11 +39249,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42432.500267129632</v>
+        <v>42432.96724953704</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42432.500267129632</v>
+        <v>42432.96724953704</v>
       </c>
       <c r="D2" t="s">
         <v>1104</v>
@@ -39265,11 +39265,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42432.500267129632</v>
+        <v>42432.96724953704</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42432.500267129632</v>
+        <v>42432.96724953704</v>
       </c>
       <c r="D3" t="s">
         <v>1104</v>
@@ -39284,8 +39284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -39295,7 +39295,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="C1" t="s">
         <v>1108</v>
@@ -39306,10 +39306,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="C2" t="s">
-        <v>1109</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -39317,10 +39317,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C3" t="s">
-        <v>1111</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -39328,10 +39328,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>1113</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31" x14ac:dyDescent="0.35">
@@ -41399,10 +41399,10 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>16</v>
@@ -41431,7 +41431,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -41457,7 +41457,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -41465,7 +41465,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>24</v>
@@ -41509,7 +41509,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -41535,7 +41535,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -41587,7 +41587,7 @@
         <v>0.8</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -41743,7 +41743,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -41751,7 +41751,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>60</v>
@@ -42055,7 +42055,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -42107,7 +42107,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -42115,13 +42115,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>1122</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>1125</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>26</v>
@@ -42133,7 +42133,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -42156,7 +42156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -42460,7 +42460,7 @@
         <v>1039</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add campaigns to initial data
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3620" uniqueCount="2304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="2306">
   <si>
     <t>tag_name</t>
   </si>
@@ -6950,6 +6950,12 @@
   </si>
   <si>
     <t>% missed children</t>
+  </si>
+  <si>
+    <t>March 2016 - OPV - LPD</t>
+  </si>
+  <si>
+    <t>November 2015 - OPV - LPD</t>
   </si>
 </sst>
 </file>
@@ -42951,11 +42957,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.533880555558</v>
+        <v>42487.817650694444</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.533880555558</v>
+        <v>42487.817650694444</v>
       </c>
       <c r="D2" t="s">
         <v>1054</v>
@@ -42967,11 +42973,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.533880555558</v>
+        <v>42487.817650694444</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.533880555558</v>
+        <v>42487.817650694444</v>
       </c>
       <c r="D3" t="s">
         <v>1054</v>
@@ -45989,7 +45995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
@@ -81417,10 +81423,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -81557,6 +81563,58 @@
         <v>1</v>
       </c>
       <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>42430</v>
+      </c>
+      <c r="C6" s="12">
+        <v>42430</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2304</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>42309</v>
+      </c>
+      <c r="C7" s="12">
+        <v>42316</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2305</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
     </row>

</xml_diff>